<commit_message>
update wrong data in database
</commit_message>
<xml_diff>
--- a/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
+++ b/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="75">
   <si>
     <t>TS</t>
   </si>
@@ -249,21 +249,6 @@
   </si>
   <si>
     <t>- Thị giác máy tính</t>
-  </si>
-  <si>
-    <t>CHƯƠNG TRÌNH ĐÀO TẠO CÔNG NGHỆ THÔNG TIN KHÓA 2021</t>
-  </si>
-  <si>
-    <t>CHƯƠNG TRÌNH ĐÀO TẠO CÔNG NGHỆ THÔNG TIN KHÓA 2022</t>
-  </si>
-  <si>
-    <t>CHƯƠNG TRÌNH ĐÀO TẠO CÔNG NGHỆ THÔNG TIN KHÓA 2023</t>
-  </si>
-  <si>
-    <t>CHƯƠNG TRÌNH ĐÀO TẠO CÔNG NGHỆ THÔNG TIN KHÓA 2025</t>
-  </si>
-  <si>
-    <t>CHƯƠNG TRÌNH ĐÀO TẠO CÔNG NGHỆ THÔNG TIN KHÓA 2026</t>
   </si>
 </sst>
 </file>
@@ -452,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -493,6 +478,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -512,39 +533,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -829,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,54 +833,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -907,7 +895,7 @@
       <c r="D3" s="12">
         <v>1</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="15">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -930,7 +918,7 @@
       <c r="D4" s="13">
         <v>0</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="15">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -953,7 +941,7 @@
       <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="15">
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -976,7 +964,7 @@
       <c r="D6" s="13">
         <v>1</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="15">
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -999,7 +987,7 @@
       <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="15">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1022,7 +1010,7 @@
       <c r="D8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="15">
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1045,7 +1033,7 @@
       <c r="D9" s="13">
         <v>1</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="15">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1068,7 +1056,7 @@
       <c r="D10" s="13">
         <v>2</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="15">
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1286,19 +1274,19 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="26">
-        <v>1</v>
-      </c>
-      <c r="C20" s="26">
+      <c r="B20" s="20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="20">
         <v>0</v>
       </c>
-      <c r="D20" s="27">
-        <v>1</v>
-      </c>
-      <c r="E20" s="30">
+      <c r="D20" s="21">
+        <v>1</v>
+      </c>
+      <c r="E20" s="24">
         <v>3</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -1309,19 +1297,19 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="25">
-        <v>2</v>
-      </c>
-      <c r="C21" s="25">
-        <v>2</v>
-      </c>
-      <c r="D21" s="28">
+      <c r="B21" s="19">
+        <v>2</v>
+      </c>
+      <c r="C21" s="19">
+        <v>2</v>
+      </c>
+      <c r="D21" s="22">
         <v>0</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="24">
         <v>3</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -1341,10 +1329,10 @@
       <c r="C22" s="13">
         <v>2</v>
       </c>
-      <c r="D22" s="29">
-        <v>1</v>
-      </c>
-      <c r="E22" s="30">
+      <c r="D22" s="23">
+        <v>1</v>
+      </c>
+      <c r="E22" s="24">
         <v>3</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -1364,10 +1352,10 @@
       <c r="C23" s="13">
         <v>2</v>
       </c>
-      <c r="D23" s="29">
-        <v>1</v>
-      </c>
-      <c r="E23" s="30">
+      <c r="D23" s="23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="24">
         <v>3</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -1387,10 +1375,10 @@
       <c r="C24" s="13">
         <v>2</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="23">
         <v>0</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="24">
         <v>3</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -1410,10 +1398,10 @@
       <c r="C25" s="13">
         <v>2</v>
       </c>
-      <c r="D25" s="29">
-        <v>1</v>
-      </c>
-      <c r="E25" s="30">
+      <c r="D25" s="23">
+        <v>1</v>
+      </c>
+      <c r="E25" s="24">
         <v>3</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -1433,10 +1421,10 @@
       <c r="C26" s="13">
         <v>2</v>
       </c>
-      <c r="D26" s="29">
-        <v>1</v>
-      </c>
-      <c r="E26" s="30">
+      <c r="D26" s="23">
+        <v>1</v>
+      </c>
+      <c r="E26" s="24">
         <v>3</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -1456,10 +1444,10 @@
       <c r="C27" s="13">
         <v>2</v>
       </c>
-      <c r="D27" s="29">
-        <v>1</v>
-      </c>
-      <c r="E27" s="30">
+      <c r="D27" s="23">
+        <v>1</v>
+      </c>
+      <c r="E27" s="24">
         <v>3</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -1479,10 +1467,10 @@
       <c r="C28" s="13">
         <v>2</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="23">
         <v>0</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="24">
         <v>4</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -1502,10 +1490,10 @@
       <c r="C29" s="13">
         <v>2</v>
       </c>
-      <c r="D29" s="29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="30">
+      <c r="D29" s="23">
+        <v>1</v>
+      </c>
+      <c r="E29" s="24">
         <v>4</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -1525,10 +1513,10 @@
       <c r="C30" s="13">
         <v>2</v>
       </c>
-      <c r="D30" s="29">
-        <v>1</v>
-      </c>
-      <c r="E30" s="30">
+      <c r="D30" s="23">
+        <v>1</v>
+      </c>
+      <c r="E30" s="24">
         <v>4</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -1548,10 +1536,10 @@
       <c r="C31" s="13">
         <v>2</v>
       </c>
-      <c r="D31" s="29">
-        <v>1</v>
-      </c>
-      <c r="E31" s="30">
+      <c r="D31" s="23">
+        <v>1</v>
+      </c>
+      <c r="E31" s="24">
         <v>4</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -1571,10 +1559,10 @@
       <c r="C32" s="13">
         <v>2</v>
       </c>
-      <c r="D32" s="29">
-        <v>1</v>
-      </c>
-      <c r="E32" s="30">
+      <c r="D32" s="23">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24">
         <v>4</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -1594,10 +1582,10 @@
       <c r="C33" s="13">
         <v>2</v>
       </c>
-      <c r="D33" s="29">
-        <v>1</v>
-      </c>
-      <c r="E33" s="30">
+      <c r="D33" s="23">
+        <v>1</v>
+      </c>
+      <c r="E33" s="24">
         <v>4</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -1617,10 +1605,10 @@
       <c r="C34" s="13">
         <v>1</v>
       </c>
-      <c r="D34" s="29">
-        <v>1</v>
-      </c>
-      <c r="E34" s="30">
+      <c r="D34" s="23">
+        <v>1</v>
+      </c>
+      <c r="E34" s="24">
         <v>4</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -1640,10 +1628,10 @@
       <c r="C35" s="13">
         <v>1</v>
       </c>
-      <c r="D35" s="29">
-        <v>1</v>
-      </c>
-      <c r="E35" s="30">
+      <c r="D35" s="23">
+        <v>1</v>
+      </c>
+      <c r="E35" s="24">
         <v>4</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -1663,10 +1651,10 @@
       <c r="C36" s="13">
         <v>1</v>
       </c>
-      <c r="D36" s="29">
-        <v>1</v>
-      </c>
-      <c r="E36" s="30">
+      <c r="D36" s="23">
+        <v>1</v>
+      </c>
+      <c r="E36" s="24">
         <v>4</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -1677,19 +1665,19 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="25">
-        <v>2</v>
-      </c>
-      <c r="C37" s="25">
-        <v>2</v>
-      </c>
-      <c r="D37" s="28">
+      <c r="B37" s="19">
+        <v>2</v>
+      </c>
+      <c r="C37" s="19">
+        <v>2</v>
+      </c>
+      <c r="D37" s="22">
         <v>0</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="24">
         <v>5</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1700,19 +1688,19 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="25">
-        <v>3</v>
-      </c>
-      <c r="C38" s="25">
-        <v>2</v>
-      </c>
-      <c r="D38" s="28">
-        <v>1</v>
-      </c>
-      <c r="E38" s="30">
+      <c r="B38" s="19">
+        <v>3</v>
+      </c>
+      <c r="C38" s="19">
+        <v>2</v>
+      </c>
+      <c r="D38" s="22">
+        <v>1</v>
+      </c>
+      <c r="E38" s="24">
         <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -1723,19 +1711,19 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="25">
-        <v>3</v>
-      </c>
-      <c r="C39" s="25">
+      <c r="B39" s="19">
+        <v>3</v>
+      </c>
+      <c r="C39" s="19">
         <v>0</v>
       </c>
-      <c r="D39" s="28">
-        <v>3</v>
-      </c>
-      <c r="E39" s="30">
+      <c r="D39" s="22">
+        <v>3</v>
+      </c>
+      <c r="E39" s="24">
         <v>5</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -1746,19 +1734,19 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="25">
-        <v>3</v>
-      </c>
-      <c r="C40" s="25">
-        <v>2</v>
-      </c>
-      <c r="D40" s="28">
-        <v>1</v>
-      </c>
-      <c r="E40" s="30">
+      <c r="B40" s="19">
+        <v>3</v>
+      </c>
+      <c r="C40" s="19">
+        <v>2</v>
+      </c>
+      <c r="D40" s="22">
+        <v>1</v>
+      </c>
+      <c r="E40" s="24">
         <v>5</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -1769,19 +1757,19 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="25">
-        <v>3</v>
-      </c>
-      <c r="C41" s="25">
-        <v>2</v>
-      </c>
-      <c r="D41" s="28">
-        <v>1</v>
-      </c>
-      <c r="E41" s="30">
+      <c r="B41" s="19">
+        <v>3</v>
+      </c>
+      <c r="C41" s="19">
+        <v>2</v>
+      </c>
+      <c r="D41" s="22">
+        <v>1</v>
+      </c>
+      <c r="E41" s="24">
         <v>5</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -1792,19 +1780,19 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="25">
-        <v>3</v>
-      </c>
-      <c r="C42" s="25">
-        <v>2</v>
-      </c>
-      <c r="D42" s="28">
-        <v>1</v>
-      </c>
-      <c r="E42" s="30">
+      <c r="B42" s="19">
+        <v>3</v>
+      </c>
+      <c r="C42" s="19">
+        <v>2</v>
+      </c>
+      <c r="D42" s="22">
+        <v>1</v>
+      </c>
+      <c r="E42" s="24">
         <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
@@ -1815,19 +1803,19 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="25">
-        <v>3</v>
-      </c>
-      <c r="C43" s="25">
-        <v>2</v>
-      </c>
-      <c r="D43" s="28">
-        <v>1</v>
-      </c>
-      <c r="E43" s="30">
+      <c r="B43" s="19">
+        <v>3</v>
+      </c>
+      <c r="C43" s="19">
+        <v>2</v>
+      </c>
+      <c r="D43" s="22">
+        <v>1</v>
+      </c>
+      <c r="E43" s="24">
         <v>5</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -1838,19 +1826,19 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="25">
-        <v>3</v>
-      </c>
-      <c r="C44" s="25">
-        <v>2</v>
-      </c>
-      <c r="D44" s="28">
-        <v>1</v>
-      </c>
-      <c r="E44" s="30">
+      <c r="B44" s="19">
+        <v>3</v>
+      </c>
+      <c r="C44" s="19">
+        <v>2</v>
+      </c>
+      <c r="D44" s="22">
+        <v>1</v>
+      </c>
+      <c r="E44" s="24">
         <v>5</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -1870,10 +1858,10 @@
       <c r="C45" s="13">
         <v>2</v>
       </c>
-      <c r="D45" s="29">
-        <v>1</v>
-      </c>
-      <c r="E45" s="30">
+      <c r="D45" s="23">
+        <v>1</v>
+      </c>
+      <c r="E45" s="24">
         <v>6</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -1893,10 +1881,10 @@
       <c r="C46" s="13">
         <v>2</v>
       </c>
-      <c r="D46" s="29">
-        <v>1</v>
-      </c>
-      <c r="E46" s="30">
+      <c r="D46" s="23">
+        <v>1</v>
+      </c>
+      <c r="E46" s="24">
         <v>6</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -1916,10 +1904,10 @@
       <c r="C47" s="13">
         <v>2</v>
       </c>
-      <c r="D47" s="29">
-        <v>1</v>
-      </c>
-      <c r="E47" s="30">
+      <c r="D47" s="23">
+        <v>1</v>
+      </c>
+      <c r="E47" s="24">
         <v>6</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -1939,10 +1927,10 @@
       <c r="C48" s="13">
         <v>2</v>
       </c>
-      <c r="D48" s="29">
-        <v>1</v>
-      </c>
-      <c r="E48" s="30">
+      <c r="D48" s="23">
+        <v>1</v>
+      </c>
+      <c r="E48" s="24">
         <v>6</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -1962,10 +1950,10 @@
       <c r="C49" s="13">
         <v>2</v>
       </c>
-      <c r="D49" s="29">
-        <v>1</v>
-      </c>
-      <c r="E49" s="30">
+      <c r="D49" s="23">
+        <v>1</v>
+      </c>
+      <c r="E49" s="24">
         <v>6</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -1985,10 +1973,10 @@
       <c r="C50" s="13">
         <v>2</v>
       </c>
-      <c r="D50" s="29">
-        <v>1</v>
-      </c>
-      <c r="E50" s="30">
+      <c r="D50" s="23">
+        <v>1</v>
+      </c>
+      <c r="E50" s="24">
         <v>6</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -2008,10 +1996,10 @@
       <c r="C51" s="13">
         <v>1</v>
       </c>
-      <c r="D51" s="29">
-        <v>1</v>
-      </c>
-      <c r="E51" s="30">
+      <c r="D51" s="23">
+        <v>1</v>
+      </c>
+      <c r="E51" s="24">
         <v>6</v>
       </c>
       <c r="F51" s="3" t="s">
@@ -2031,10 +2019,10 @@
       <c r="C52" s="13">
         <v>1</v>
       </c>
-      <c r="D52" s="29">
-        <v>1</v>
-      </c>
-      <c r="E52" s="30">
+      <c r="D52" s="23">
+        <v>1</v>
+      </c>
+      <c r="E52" s="24">
         <v>6</v>
       </c>
       <c r="F52" s="3" t="s">
@@ -2054,10 +2042,10 @@
       <c r="C53" s="13">
         <v>1</v>
       </c>
-      <c r="D53" s="29">
-        <v>1</v>
-      </c>
-      <c r="E53" s="30">
+      <c r="D53" s="23">
+        <v>1</v>
+      </c>
+      <c r="E53" s="24">
         <v>6</v>
       </c>
       <c r="F53" s="3" t="s">
@@ -2077,10 +2065,10 @@
       <c r="C54" s="13">
         <v>1</v>
       </c>
-      <c r="D54" s="29">
-        <v>1</v>
-      </c>
-      <c r="E54" s="30">
+      <c r="D54" s="23">
+        <v>1</v>
+      </c>
+      <c r="E54" s="24">
         <v>6</v>
       </c>
       <c r="F54" s="3" t="s">
@@ -2091,19 +2079,19 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="25">
-        <v>3</v>
-      </c>
-      <c r="C55" s="25">
-        <v>2</v>
-      </c>
-      <c r="D55" s="28">
-        <v>1</v>
-      </c>
-      <c r="E55" s="30">
+      <c r="B55" s="19">
+        <v>3</v>
+      </c>
+      <c r="C55" s="19">
+        <v>2</v>
+      </c>
+      <c r="D55" s="22">
+        <v>1</v>
+      </c>
+      <c r="E55" s="24">
         <v>7</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -2123,10 +2111,10 @@
       <c r="C56" s="13">
         <v>2</v>
       </c>
-      <c r="D56" s="29">
-        <v>1</v>
-      </c>
-      <c r="E56" s="30">
+      <c r="D56" s="23">
+        <v>1</v>
+      </c>
+      <c r="E56" s="24">
         <v>7</v>
       </c>
       <c r="F56" s="3" t="s">
@@ -2146,10 +2134,10 @@
       <c r="C57" s="13">
         <v>2</v>
       </c>
-      <c r="D57" s="29">
-        <v>1</v>
-      </c>
-      <c r="E57" s="30">
+      <c r="D57" s="23">
+        <v>1</v>
+      </c>
+      <c r="E57" s="24">
         <v>7</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -2169,10 +2157,10 @@
       <c r="C58" s="13">
         <v>0</v>
       </c>
-      <c r="D58" s="29">
-        <v>3</v>
-      </c>
-      <c r="E58" s="30">
+      <c r="D58" s="23">
+        <v>3</v>
+      </c>
+      <c r="E58" s="24">
         <v>7</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -2192,10 +2180,10 @@
       <c r="C59" s="13">
         <v>2</v>
       </c>
-      <c r="D59" s="29">
-        <v>1</v>
-      </c>
-      <c r="E59" s="30">
+      <c r="D59" s="23">
+        <v>1</v>
+      </c>
+      <c r="E59" s="24">
         <v>7</v>
       </c>
       <c r="F59" s="3" t="s">
@@ -2215,10 +2203,10 @@
       <c r="C60" s="13">
         <v>2</v>
       </c>
-      <c r="D60" s="29">
-        <v>1</v>
-      </c>
-      <c r="E60" s="30">
+      <c r="D60" s="23">
+        <v>1</v>
+      </c>
+      <c r="E60" s="24">
         <v>7</v>
       </c>
       <c r="F60" s="3" t="s">
@@ -2238,10 +2226,10 @@
       <c r="C61" s="13">
         <v>2</v>
       </c>
-      <c r="D61" s="29">
-        <v>1</v>
-      </c>
-      <c r="E61" s="30">
+      <c r="D61" s="23">
+        <v>1</v>
+      </c>
+      <c r="E61" s="24">
         <v>7</v>
       </c>
       <c r="F61" s="3" t="s">
@@ -2261,10 +2249,10 @@
       <c r="C62" s="13">
         <v>2</v>
       </c>
-      <c r="D62" s="29">
-        <v>1</v>
-      </c>
-      <c r="E62" s="30">
+      <c r="D62" s="23">
+        <v>1</v>
+      </c>
+      <c r="E62" s="24">
         <v>7</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -2284,10 +2272,10 @@
       <c r="C63" s="13">
         <v>2</v>
       </c>
-      <c r="D63" s="29">
-        <v>1</v>
-      </c>
-      <c r="E63" s="30">
+      <c r="D63" s="23">
+        <v>1</v>
+      </c>
+      <c r="E63" s="24">
         <v>7</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -2310,14 +2298,14 @@
       <c r="D64" s="13">
         <v>1</v>
       </c>
-      <c r="E64" s="24">
+      <c r="E64" s="18">
         <v>8</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G64" s="8" t="s">
-        <v>75</v>
+      <c r="G64" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -2333,14 +2321,14 @@
       <c r="D65" s="13">
         <v>3</v>
       </c>
-      <c r="E65" s="31">
+      <c r="E65" s="25">
         <v>8</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G65" s="8" t="s">
-        <v>76</v>
+      <c r="G65" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -2356,14 +2344,14 @@
       <c r="D66" s="13">
         <v>7</v>
       </c>
-      <c r="E66" s="24">
+      <c r="E66" s="18">
         <v>8</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G66" s="8" t="s">
-        <v>77</v>
+      <c r="G66" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -2379,14 +2367,14 @@
       <c r="D67" s="13">
         <v>1</v>
       </c>
-      <c r="E67" s="24">
+      <c r="E67" s="18">
         <v>8</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G67" s="8" t="s">
-        <v>78</v>
+      <c r="G67" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -2402,14 +2390,14 @@
       <c r="D68" s="13">
         <v>2</v>
       </c>
-      <c r="E68" s="31">
+      <c r="E68" s="25">
         <v>8</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G68" s="8" t="s">
-        <v>79</v>
+      <c r="G68" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add api lop : select and create
</commit_message>
<xml_diff>
--- a/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
+++ b/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\NghienCuuKhoaHoc\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -248,7 +248,7 @@
     <t>- Thị giác máy tính</t>
   </si>
   <si>
-    <t xml:space="preserve"> CÔNG NGHỆ THÔNG TIN KHÓA 2020</t>
+    <t>CÔNG NGHỆ THÔNG TIN KHÓA 2020</t>
   </si>
 </sst>
 </file>
@@ -508,6 +508,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -516,18 +528,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G68"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,54 +827,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
     </row>
     <row r="2" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -2396,11 +2396,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
@@ -2412,6 +2407,11 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add file excel bên folder Tài liệu
</commit_message>
<xml_diff>
--- a/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
+++ b/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\NghienCuuKhoaHoc\Tài liệu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="77">
   <si>
     <t>TS</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>CÔNG NGHỆ THÔNG TIN KHÓA 2020</t>
+  </si>
+  <si>
+    <t>CÔNG NGHỆ THÔNG TIN KHÓA 2021</t>
+  </si>
+  <si>
+    <t>CÔNG NGHỆ THÔNG TIN KHÓA 2022</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -507,6 +513,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -809,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,54 +836,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -2392,6 +2401,3042 @@
       </c>
       <c r="G68" s="23" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="10">
+        <v>1</v>
+      </c>
+      <c r="C69" s="9">
+        <v>0</v>
+      </c>
+      <c r="D69" s="10">
+        <v>1</v>
+      </c>
+      <c r="E69" s="12">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" s="11">
+        <v>3</v>
+      </c>
+      <c r="C70" s="11">
+        <v>3</v>
+      </c>
+      <c r="D70" s="11">
+        <v>0</v>
+      </c>
+      <c r="E70" s="12">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="11">
+        <v>3</v>
+      </c>
+      <c r="C71" s="11">
+        <v>2</v>
+      </c>
+      <c r="D71" s="11">
+        <v>1</v>
+      </c>
+      <c r="E71" s="12">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="11">
+        <v>2</v>
+      </c>
+      <c r="C72" s="11">
+        <v>1</v>
+      </c>
+      <c r="D72" s="11">
+        <v>1</v>
+      </c>
+      <c r="E72" s="12">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" s="11">
+        <v>2</v>
+      </c>
+      <c r="C73" s="11">
+        <v>1</v>
+      </c>
+      <c r="D73" s="11">
+        <v>1</v>
+      </c>
+      <c r="E73" s="12">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G73" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74" s="11">
+        <v>3</v>
+      </c>
+      <c r="C74" s="11">
+        <v>2</v>
+      </c>
+      <c r="D74" s="11">
+        <v>1</v>
+      </c>
+      <c r="E74" s="12">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="11">
+        <v>2</v>
+      </c>
+      <c r="C75" s="11">
+        <v>1</v>
+      </c>
+      <c r="D75" s="11">
+        <v>1</v>
+      </c>
+      <c r="E75" s="12">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="11">
+        <v>4</v>
+      </c>
+      <c r="C76" s="11">
+        <v>2</v>
+      </c>
+      <c r="D76" s="11">
+        <v>2</v>
+      </c>
+      <c r="E76" s="12">
+        <v>1</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="24">
+        <v>2</v>
+      </c>
+      <c r="C78" s="24">
+        <v>2</v>
+      </c>
+      <c r="D78" s="24">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>2</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="24">
+        <v>4</v>
+      </c>
+      <c r="C79" s="24">
+        <v>2</v>
+      </c>
+      <c r="D79" s="24">
+        <v>2</v>
+      </c>
+      <c r="E79" s="1">
+        <v>2</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="24">
+        <v>2</v>
+      </c>
+      <c r="C80" s="24">
+        <v>1</v>
+      </c>
+      <c r="D80" s="24">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="24">
+        <v>2</v>
+      </c>
+      <c r="C81" s="24">
+        <v>1</v>
+      </c>
+      <c r="D81" s="24">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>2</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="24">
+        <v>2</v>
+      </c>
+      <c r="C82" s="24">
+        <v>1</v>
+      </c>
+      <c r="D82" s="24">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" s="24">
+        <v>2</v>
+      </c>
+      <c r="C83" s="24">
+        <v>1</v>
+      </c>
+      <c r="D83" s="24">
+        <v>1</v>
+      </c>
+      <c r="E83" s="1">
+        <v>2</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="24">
+        <v>2</v>
+      </c>
+      <c r="C84" s="24">
+        <v>1</v>
+      </c>
+      <c r="D84" s="24">
+        <v>1</v>
+      </c>
+      <c r="E84" s="1">
+        <v>2</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="24">
+        <v>4</v>
+      </c>
+      <c r="C85" s="24">
+        <v>2</v>
+      </c>
+      <c r="D85" s="24">
+        <v>2</v>
+      </c>
+      <c r="E85" s="1">
+        <v>2</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="17">
+        <v>1</v>
+      </c>
+      <c r="C86" s="17">
+        <v>0</v>
+      </c>
+      <c r="D86" s="18">
+        <v>1</v>
+      </c>
+      <c r="E86" s="21">
+        <v>3</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G86" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="16">
+        <v>2</v>
+      </c>
+      <c r="C87" s="16">
+        <v>2</v>
+      </c>
+      <c r="D87" s="19">
+        <v>0</v>
+      </c>
+      <c r="E87" s="21">
+        <v>3</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B88" s="11">
+        <v>3</v>
+      </c>
+      <c r="C88" s="11">
+        <v>2</v>
+      </c>
+      <c r="D88" s="20">
+        <v>1</v>
+      </c>
+      <c r="E88" s="21">
+        <v>3</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" s="11">
+        <v>3</v>
+      </c>
+      <c r="C89" s="11">
+        <v>2</v>
+      </c>
+      <c r="D89" s="20">
+        <v>1</v>
+      </c>
+      <c r="E89" s="21">
+        <v>3</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B90" s="11">
+        <v>2</v>
+      </c>
+      <c r="C90" s="11">
+        <v>2</v>
+      </c>
+      <c r="D90" s="20">
+        <v>0</v>
+      </c>
+      <c r="E90" s="21">
+        <v>3</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B91" s="11">
+        <v>3</v>
+      </c>
+      <c r="C91" s="11">
+        <v>2</v>
+      </c>
+      <c r="D91" s="20">
+        <v>1</v>
+      </c>
+      <c r="E91" s="21">
+        <v>3</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B92" s="11">
+        <v>3</v>
+      </c>
+      <c r="C92" s="11">
+        <v>2</v>
+      </c>
+      <c r="D92" s="20">
+        <v>1</v>
+      </c>
+      <c r="E92" s="21">
+        <v>3</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B93" s="11">
+        <v>3</v>
+      </c>
+      <c r="C93" s="11">
+        <v>2</v>
+      </c>
+      <c r="D93" s="20">
+        <v>1</v>
+      </c>
+      <c r="E93" s="21">
+        <v>3</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B94" s="11">
+        <v>2</v>
+      </c>
+      <c r="C94" s="11">
+        <v>2</v>
+      </c>
+      <c r="D94" s="20">
+        <v>0</v>
+      </c>
+      <c r="E94" s="21">
+        <v>4</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B95" s="11">
+        <v>3</v>
+      </c>
+      <c r="C95" s="11">
+        <v>2</v>
+      </c>
+      <c r="D95" s="20">
+        <v>1</v>
+      </c>
+      <c r="E95" s="21">
+        <v>4</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B96" s="11">
+        <v>3</v>
+      </c>
+      <c r="C96" s="11">
+        <v>2</v>
+      </c>
+      <c r="D96" s="20">
+        <v>1</v>
+      </c>
+      <c r="E96" s="21">
+        <v>4</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B97" s="11">
+        <v>3</v>
+      </c>
+      <c r="C97" s="11">
+        <v>2</v>
+      </c>
+      <c r="D97" s="20">
+        <v>1</v>
+      </c>
+      <c r="E97" s="21">
+        <v>4</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B98" s="11">
+        <v>3</v>
+      </c>
+      <c r="C98" s="11">
+        <v>2</v>
+      </c>
+      <c r="D98" s="20">
+        <v>1</v>
+      </c>
+      <c r="E98" s="21">
+        <v>4</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99" s="11">
+        <v>3</v>
+      </c>
+      <c r="C99" s="11">
+        <v>2</v>
+      </c>
+      <c r="D99" s="20">
+        <v>1</v>
+      </c>
+      <c r="E99" s="21">
+        <v>4</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G99" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B100" s="11">
+        <v>2</v>
+      </c>
+      <c r="C100" s="11">
+        <v>1</v>
+      </c>
+      <c r="D100" s="20">
+        <v>1</v>
+      </c>
+      <c r="E100" s="21">
+        <v>4</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B101" s="11">
+        <v>2</v>
+      </c>
+      <c r="C101" s="11">
+        <v>1</v>
+      </c>
+      <c r="D101" s="20">
+        <v>1</v>
+      </c>
+      <c r="E101" s="21">
+        <v>4</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" s="11">
+        <v>2</v>
+      </c>
+      <c r="C102" s="11">
+        <v>1</v>
+      </c>
+      <c r="D102" s="20">
+        <v>1</v>
+      </c>
+      <c r="E102" s="21">
+        <v>4</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B103" s="16">
+        <v>2</v>
+      </c>
+      <c r="C103" s="16">
+        <v>2</v>
+      </c>
+      <c r="D103" s="19">
+        <v>0</v>
+      </c>
+      <c r="E103" s="21">
+        <v>5</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B104" s="16">
+        <v>3</v>
+      </c>
+      <c r="C104" s="16">
+        <v>2</v>
+      </c>
+      <c r="D104" s="19">
+        <v>1</v>
+      </c>
+      <c r="E104" s="21">
+        <v>5</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B105" s="16">
+        <v>3</v>
+      </c>
+      <c r="C105" s="16">
+        <v>0</v>
+      </c>
+      <c r="D105" s="19">
+        <v>3</v>
+      </c>
+      <c r="E105" s="21">
+        <v>5</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B106" s="16">
+        <v>3</v>
+      </c>
+      <c r="C106" s="16">
+        <v>2</v>
+      </c>
+      <c r="D106" s="19">
+        <v>1</v>
+      </c>
+      <c r="E106" s="21">
+        <v>5</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B107" s="16">
+        <v>3</v>
+      </c>
+      <c r="C107" s="16">
+        <v>2</v>
+      </c>
+      <c r="D107" s="19">
+        <v>1</v>
+      </c>
+      <c r="E107" s="21">
+        <v>5</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A108" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B108" s="16">
+        <v>3</v>
+      </c>
+      <c r="C108" s="16">
+        <v>2</v>
+      </c>
+      <c r="D108" s="19">
+        <v>1</v>
+      </c>
+      <c r="E108" s="21">
+        <v>5</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G108" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B109" s="16">
+        <v>3</v>
+      </c>
+      <c r="C109" s="16">
+        <v>2</v>
+      </c>
+      <c r="D109" s="19">
+        <v>1</v>
+      </c>
+      <c r="E109" s="21">
+        <v>5</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G109" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B110" s="16">
+        <v>3</v>
+      </c>
+      <c r="C110" s="16">
+        <v>2</v>
+      </c>
+      <c r="D110" s="19">
+        <v>1</v>
+      </c>
+      <c r="E110" s="21">
+        <v>5</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B111" s="11">
+        <v>3</v>
+      </c>
+      <c r="C111" s="11">
+        <v>2</v>
+      </c>
+      <c r="D111" s="20">
+        <v>1</v>
+      </c>
+      <c r="E111" s="21">
+        <v>6</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G111" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B112" s="11">
+        <v>3</v>
+      </c>
+      <c r="C112" s="11">
+        <v>2</v>
+      </c>
+      <c r="D112" s="20">
+        <v>1</v>
+      </c>
+      <c r="E112" s="21">
+        <v>6</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B113" s="11">
+        <v>3</v>
+      </c>
+      <c r="C113" s="11">
+        <v>2</v>
+      </c>
+      <c r="D113" s="20">
+        <v>1</v>
+      </c>
+      <c r="E113" s="21">
+        <v>6</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G113" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B114" s="11">
+        <v>3</v>
+      </c>
+      <c r="C114" s="11">
+        <v>2</v>
+      </c>
+      <c r="D114" s="20">
+        <v>1</v>
+      </c>
+      <c r="E114" s="21">
+        <v>6</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B115" s="11">
+        <v>3</v>
+      </c>
+      <c r="C115" s="11">
+        <v>2</v>
+      </c>
+      <c r="D115" s="20">
+        <v>1</v>
+      </c>
+      <c r="E115" s="21">
+        <v>6</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B116" s="11">
+        <v>3</v>
+      </c>
+      <c r="C116" s="11">
+        <v>2</v>
+      </c>
+      <c r="D116" s="20">
+        <v>1</v>
+      </c>
+      <c r="E116" s="21">
+        <v>6</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G116" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B117" s="11">
+        <v>2</v>
+      </c>
+      <c r="C117" s="11">
+        <v>1</v>
+      </c>
+      <c r="D117" s="20">
+        <v>1</v>
+      </c>
+      <c r="E117" s="21">
+        <v>6</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G117" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B118" s="11">
+        <v>2</v>
+      </c>
+      <c r="C118" s="11">
+        <v>1</v>
+      </c>
+      <c r="D118" s="20">
+        <v>1</v>
+      </c>
+      <c r="E118" s="21">
+        <v>6</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G118" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B119" s="11">
+        <v>2</v>
+      </c>
+      <c r="C119" s="11">
+        <v>1</v>
+      </c>
+      <c r="D119" s="20">
+        <v>1</v>
+      </c>
+      <c r="E119" s="21">
+        <v>6</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G119" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B120" s="11">
+        <v>2</v>
+      </c>
+      <c r="C120" s="11">
+        <v>1</v>
+      </c>
+      <c r="D120" s="20">
+        <v>1</v>
+      </c>
+      <c r="E120" s="21">
+        <v>6</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G120" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B121" s="16">
+        <v>3</v>
+      </c>
+      <c r="C121" s="16">
+        <v>2</v>
+      </c>
+      <c r="D121" s="19">
+        <v>1</v>
+      </c>
+      <c r="E121" s="21">
+        <v>7</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B122" s="11">
+        <v>3</v>
+      </c>
+      <c r="C122" s="11">
+        <v>2</v>
+      </c>
+      <c r="D122" s="20">
+        <v>1</v>
+      </c>
+      <c r="E122" s="21">
+        <v>7</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G122" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B123" s="11">
+        <v>3</v>
+      </c>
+      <c r="C123" s="11">
+        <v>2</v>
+      </c>
+      <c r="D123" s="20">
+        <v>1</v>
+      </c>
+      <c r="E123" s="21">
+        <v>7</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G123" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B124" s="11">
+        <v>3</v>
+      </c>
+      <c r="C124" s="11">
+        <v>0</v>
+      </c>
+      <c r="D124" s="20">
+        <v>3</v>
+      </c>
+      <c r="E124" s="21">
+        <v>7</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A125" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B125" s="11">
+        <v>3</v>
+      </c>
+      <c r="C125" s="11">
+        <v>2</v>
+      </c>
+      <c r="D125" s="20">
+        <v>1</v>
+      </c>
+      <c r="E125" s="21">
+        <v>7</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G125" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B126" s="11">
+        <v>3</v>
+      </c>
+      <c r="C126" s="11">
+        <v>2</v>
+      </c>
+      <c r="D126" s="20">
+        <v>1</v>
+      </c>
+      <c r="E126" s="21">
+        <v>7</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G126" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B127" s="11">
+        <v>3</v>
+      </c>
+      <c r="C127" s="11">
+        <v>2</v>
+      </c>
+      <c r="D127" s="20">
+        <v>1</v>
+      </c>
+      <c r="E127" s="21">
+        <v>7</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G127" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B128" s="11">
+        <v>3</v>
+      </c>
+      <c r="C128" s="11">
+        <v>2</v>
+      </c>
+      <c r="D128" s="20">
+        <v>1</v>
+      </c>
+      <c r="E128" s="21">
+        <v>7</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G128" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B129" s="11">
+        <v>3</v>
+      </c>
+      <c r="C129" s="11">
+        <v>2</v>
+      </c>
+      <c r="D129" s="20">
+        <v>1</v>
+      </c>
+      <c r="E129" s="21">
+        <v>7</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G129" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B130" s="11">
+        <v>3</v>
+      </c>
+      <c r="C130" s="11">
+        <v>2</v>
+      </c>
+      <c r="D130" s="11">
+        <v>1</v>
+      </c>
+      <c r="E130" s="15">
+        <v>8</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G130" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A131" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B131" s="11">
+        <v>3</v>
+      </c>
+      <c r="C131" s="11">
+        <v>0</v>
+      </c>
+      <c r="D131" s="11">
+        <v>3</v>
+      </c>
+      <c r="E131" s="22">
+        <v>8</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G131" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B132" s="11">
+        <v>7</v>
+      </c>
+      <c r="C132" s="11">
+        <v>0</v>
+      </c>
+      <c r="D132" s="11">
+        <v>7</v>
+      </c>
+      <c r="E132" s="15">
+        <v>8</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B133" s="11">
+        <v>3</v>
+      </c>
+      <c r="C133" s="11">
+        <v>2</v>
+      </c>
+      <c r="D133" s="11">
+        <v>1</v>
+      </c>
+      <c r="E133" s="15">
+        <v>8</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G133" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B134" s="11">
+        <v>4</v>
+      </c>
+      <c r="C134" s="11">
+        <v>2</v>
+      </c>
+      <c r="D134" s="11">
+        <v>2</v>
+      </c>
+      <c r="E134" s="22">
+        <v>8</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G134" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B135" s="10">
+        <v>1</v>
+      </c>
+      <c r="C135" s="9">
+        <v>0</v>
+      </c>
+      <c r="D135" s="10">
+        <v>1</v>
+      </c>
+      <c r="E135" s="12">
+        <v>1</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" s="11">
+        <v>3</v>
+      </c>
+      <c r="C136" s="11">
+        <v>3</v>
+      </c>
+      <c r="D136" s="11">
+        <v>0</v>
+      </c>
+      <c r="E136" s="12">
+        <v>1</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A137" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B137" s="11">
+        <v>3</v>
+      </c>
+      <c r="C137" s="11">
+        <v>2</v>
+      </c>
+      <c r="D137" s="11">
+        <v>1</v>
+      </c>
+      <c r="E137" s="12">
+        <v>1</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G137" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B138" s="11">
+        <v>2</v>
+      </c>
+      <c r="C138" s="11">
+        <v>1</v>
+      </c>
+      <c r="D138" s="11">
+        <v>1</v>
+      </c>
+      <c r="E138" s="12">
+        <v>1</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G138" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B139" s="11">
+        <v>2</v>
+      </c>
+      <c r="C139" s="11">
+        <v>1</v>
+      </c>
+      <c r="D139" s="11">
+        <v>1</v>
+      </c>
+      <c r="E139" s="12">
+        <v>1</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G139" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A140" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B140" s="11">
+        <v>3</v>
+      </c>
+      <c r="C140" s="11">
+        <v>2</v>
+      </c>
+      <c r="D140" s="11">
+        <v>1</v>
+      </c>
+      <c r="E140" s="12">
+        <v>1</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G140" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B141" s="11">
+        <v>2</v>
+      </c>
+      <c r="C141" s="11">
+        <v>1</v>
+      </c>
+      <c r="D141" s="11">
+        <v>1</v>
+      </c>
+      <c r="E141" s="12">
+        <v>1</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G141" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B142" s="11">
+        <v>4</v>
+      </c>
+      <c r="C142" s="11">
+        <v>2</v>
+      </c>
+      <c r="D142" s="11">
+        <v>2</v>
+      </c>
+      <c r="E142" s="12">
+        <v>1</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G142" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B143" s="2">
+        <v>1</v>
+      </c>
+      <c r="C143" s="2">
+        <v>0</v>
+      </c>
+      <c r="D143" s="2">
+        <v>1</v>
+      </c>
+      <c r="E143" s="1">
+        <v>2</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G143" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B144" s="24">
+        <v>2</v>
+      </c>
+      <c r="C144" s="24">
+        <v>2</v>
+      </c>
+      <c r="D144" s="24">
+        <v>0</v>
+      </c>
+      <c r="E144" s="1">
+        <v>2</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G144" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B145" s="24">
+        <v>4</v>
+      </c>
+      <c r="C145" s="24">
+        <v>2</v>
+      </c>
+      <c r="D145" s="24">
+        <v>2</v>
+      </c>
+      <c r="E145" s="1">
+        <v>2</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G145" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146" s="24">
+        <v>2</v>
+      </c>
+      <c r="C146" s="24">
+        <v>1</v>
+      </c>
+      <c r="D146" s="24">
+        <v>1</v>
+      </c>
+      <c r="E146" s="1">
+        <v>2</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G146" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" s="24">
+        <v>2</v>
+      </c>
+      <c r="C147" s="24">
+        <v>1</v>
+      </c>
+      <c r="D147" s="24">
+        <v>1</v>
+      </c>
+      <c r="E147" s="1">
+        <v>2</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G147" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" s="24">
+        <v>2</v>
+      </c>
+      <c r="C148" s="24">
+        <v>1</v>
+      </c>
+      <c r="D148" s="24">
+        <v>1</v>
+      </c>
+      <c r="E148" s="1">
+        <v>2</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G148" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B149" s="24">
+        <v>2</v>
+      </c>
+      <c r="C149" s="24">
+        <v>1</v>
+      </c>
+      <c r="D149" s="24">
+        <v>1</v>
+      </c>
+      <c r="E149" s="1">
+        <v>2</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G149" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" s="24">
+        <v>2</v>
+      </c>
+      <c r="C150" s="24">
+        <v>1</v>
+      </c>
+      <c r="D150" s="24">
+        <v>1</v>
+      </c>
+      <c r="E150" s="1">
+        <v>2</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G150" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B151" s="24">
+        <v>4</v>
+      </c>
+      <c r="C151" s="24">
+        <v>2</v>
+      </c>
+      <c r="D151" s="24">
+        <v>2</v>
+      </c>
+      <c r="E151" s="1">
+        <v>2</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G151" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A152" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B152" s="17">
+        <v>1</v>
+      </c>
+      <c r="C152" s="17">
+        <v>0</v>
+      </c>
+      <c r="D152" s="18">
+        <v>1</v>
+      </c>
+      <c r="E152" s="21">
+        <v>3</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" s="16">
+        <v>2</v>
+      </c>
+      <c r="C153" s="16">
+        <v>2</v>
+      </c>
+      <c r="D153" s="19">
+        <v>0</v>
+      </c>
+      <c r="E153" s="21">
+        <v>3</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G153" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B154" s="11">
+        <v>3</v>
+      </c>
+      <c r="C154" s="11">
+        <v>2</v>
+      </c>
+      <c r="D154" s="20">
+        <v>1</v>
+      </c>
+      <c r="E154" s="21">
+        <v>3</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G154" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A155" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B155" s="11">
+        <v>3</v>
+      </c>
+      <c r="C155" s="11">
+        <v>2</v>
+      </c>
+      <c r="D155" s="20">
+        <v>1</v>
+      </c>
+      <c r="E155" s="21">
+        <v>3</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G155" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B156" s="11">
+        <v>2</v>
+      </c>
+      <c r="C156" s="11">
+        <v>2</v>
+      </c>
+      <c r="D156" s="20">
+        <v>0</v>
+      </c>
+      <c r="E156" s="21">
+        <v>3</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G156" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A157" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B157" s="11">
+        <v>3</v>
+      </c>
+      <c r="C157" s="11">
+        <v>2</v>
+      </c>
+      <c r="D157" s="20">
+        <v>1</v>
+      </c>
+      <c r="E157" s="21">
+        <v>3</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G157" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A158" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B158" s="11">
+        <v>3</v>
+      </c>
+      <c r="C158" s="11">
+        <v>2</v>
+      </c>
+      <c r="D158" s="20">
+        <v>1</v>
+      </c>
+      <c r="E158" s="21">
+        <v>3</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G158" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A159" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B159" s="11">
+        <v>3</v>
+      </c>
+      <c r="C159" s="11">
+        <v>2</v>
+      </c>
+      <c r="D159" s="20">
+        <v>1</v>
+      </c>
+      <c r="E159" s="21">
+        <v>3</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G159" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A160" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B160" s="11">
+        <v>2</v>
+      </c>
+      <c r="C160" s="11">
+        <v>2</v>
+      </c>
+      <c r="D160" s="20">
+        <v>0</v>
+      </c>
+      <c r="E160" s="21">
+        <v>4</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G160" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A161" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B161" s="11">
+        <v>3</v>
+      </c>
+      <c r="C161" s="11">
+        <v>2</v>
+      </c>
+      <c r="D161" s="20">
+        <v>1</v>
+      </c>
+      <c r="E161" s="21">
+        <v>4</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G161" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A162" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B162" s="11">
+        <v>3</v>
+      </c>
+      <c r="C162" s="11">
+        <v>2</v>
+      </c>
+      <c r="D162" s="20">
+        <v>1</v>
+      </c>
+      <c r="E162" s="21">
+        <v>4</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G162" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A163" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B163" s="11">
+        <v>3</v>
+      </c>
+      <c r="C163" s="11">
+        <v>2</v>
+      </c>
+      <c r="D163" s="20">
+        <v>1</v>
+      </c>
+      <c r="E163" s="21">
+        <v>4</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G163" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A164" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B164" s="11">
+        <v>3</v>
+      </c>
+      <c r="C164" s="11">
+        <v>2</v>
+      </c>
+      <c r="D164" s="20">
+        <v>1</v>
+      </c>
+      <c r="E164" s="21">
+        <v>4</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G164" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A165" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B165" s="11">
+        <v>3</v>
+      </c>
+      <c r="C165" s="11">
+        <v>2</v>
+      </c>
+      <c r="D165" s="20">
+        <v>1</v>
+      </c>
+      <c r="E165" s="21">
+        <v>4</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G165" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A166" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B166" s="11">
+        <v>2</v>
+      </c>
+      <c r="C166" s="11">
+        <v>1</v>
+      </c>
+      <c r="D166" s="20">
+        <v>1</v>
+      </c>
+      <c r="E166" s="21">
+        <v>4</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G166" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A167" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B167" s="11">
+        <v>2</v>
+      </c>
+      <c r="C167" s="11">
+        <v>1</v>
+      </c>
+      <c r="D167" s="20">
+        <v>1</v>
+      </c>
+      <c r="E167" s="21">
+        <v>4</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G167" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A168" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B168" s="11">
+        <v>2</v>
+      </c>
+      <c r="C168" s="11">
+        <v>1</v>
+      </c>
+      <c r="D168" s="20">
+        <v>1</v>
+      </c>
+      <c r="E168" s="21">
+        <v>4</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G168" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B169" s="16">
+        <v>2</v>
+      </c>
+      <c r="C169" s="16">
+        <v>2</v>
+      </c>
+      <c r="D169" s="19">
+        <v>0</v>
+      </c>
+      <c r="E169" s="21">
+        <v>5</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G169" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B170" s="16">
+        <v>3</v>
+      </c>
+      <c r="C170" s="16">
+        <v>2</v>
+      </c>
+      <c r="D170" s="19">
+        <v>1</v>
+      </c>
+      <c r="E170" s="21">
+        <v>5</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G170" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B171" s="16">
+        <v>3</v>
+      </c>
+      <c r="C171" s="16">
+        <v>0</v>
+      </c>
+      <c r="D171" s="19">
+        <v>3</v>
+      </c>
+      <c r="E171" s="21">
+        <v>5</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G171" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B172" s="16">
+        <v>3</v>
+      </c>
+      <c r="C172" s="16">
+        <v>2</v>
+      </c>
+      <c r="D172" s="19">
+        <v>1</v>
+      </c>
+      <c r="E172" s="21">
+        <v>5</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G172" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B173" s="16">
+        <v>3</v>
+      </c>
+      <c r="C173" s="16">
+        <v>2</v>
+      </c>
+      <c r="D173" s="19">
+        <v>1</v>
+      </c>
+      <c r="E173" s="21">
+        <v>5</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G173" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B174" s="16">
+        <v>3</v>
+      </c>
+      <c r="C174" s="16">
+        <v>2</v>
+      </c>
+      <c r="D174" s="19">
+        <v>1</v>
+      </c>
+      <c r="E174" s="21">
+        <v>5</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G174" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B175" s="16">
+        <v>3</v>
+      </c>
+      <c r="C175" s="16">
+        <v>2</v>
+      </c>
+      <c r="D175" s="19">
+        <v>1</v>
+      </c>
+      <c r="E175" s="21">
+        <v>5</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G175" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B176" s="16">
+        <v>3</v>
+      </c>
+      <c r="C176" s="16">
+        <v>2</v>
+      </c>
+      <c r="D176" s="19">
+        <v>1</v>
+      </c>
+      <c r="E176" s="21">
+        <v>5</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G176" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A177" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B177" s="11">
+        <v>3</v>
+      </c>
+      <c r="C177" s="11">
+        <v>2</v>
+      </c>
+      <c r="D177" s="20">
+        <v>1</v>
+      </c>
+      <c r="E177" s="21">
+        <v>6</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G177" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A178" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B178" s="11">
+        <v>3</v>
+      </c>
+      <c r="C178" s="11">
+        <v>2</v>
+      </c>
+      <c r="D178" s="20">
+        <v>1</v>
+      </c>
+      <c r="E178" s="21">
+        <v>6</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G178" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A179" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B179" s="11">
+        <v>3</v>
+      </c>
+      <c r="C179" s="11">
+        <v>2</v>
+      </c>
+      <c r="D179" s="20">
+        <v>1</v>
+      </c>
+      <c r="E179" s="21">
+        <v>6</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G179" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A180" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B180" s="11">
+        <v>3</v>
+      </c>
+      <c r="C180" s="11">
+        <v>2</v>
+      </c>
+      <c r="D180" s="20">
+        <v>1</v>
+      </c>
+      <c r="E180" s="21">
+        <v>6</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G180" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A181" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B181" s="11">
+        <v>3</v>
+      </c>
+      <c r="C181" s="11">
+        <v>2</v>
+      </c>
+      <c r="D181" s="20">
+        <v>1</v>
+      </c>
+      <c r="E181" s="21">
+        <v>6</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G181" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A182" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B182" s="11">
+        <v>3</v>
+      </c>
+      <c r="C182" s="11">
+        <v>2</v>
+      </c>
+      <c r="D182" s="20">
+        <v>1</v>
+      </c>
+      <c r="E182" s="21">
+        <v>6</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G182" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A183" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B183" s="11">
+        <v>2</v>
+      </c>
+      <c r="C183" s="11">
+        <v>1</v>
+      </c>
+      <c r="D183" s="20">
+        <v>1</v>
+      </c>
+      <c r="E183" s="21">
+        <v>6</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G183" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A184" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B184" s="11">
+        <v>2</v>
+      </c>
+      <c r="C184" s="11">
+        <v>1</v>
+      </c>
+      <c r="D184" s="20">
+        <v>1</v>
+      </c>
+      <c r="E184" s="21">
+        <v>6</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G184" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A185" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B185" s="11">
+        <v>2</v>
+      </c>
+      <c r="C185" s="11">
+        <v>1</v>
+      </c>
+      <c r="D185" s="20">
+        <v>1</v>
+      </c>
+      <c r="E185" s="21">
+        <v>6</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G185" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A186" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B186" s="11">
+        <v>2</v>
+      </c>
+      <c r="C186" s="11">
+        <v>1</v>
+      </c>
+      <c r="D186" s="20">
+        <v>1</v>
+      </c>
+      <c r="E186" s="21">
+        <v>6</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G186" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A187" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B187" s="16">
+        <v>3</v>
+      </c>
+      <c r="C187" s="16">
+        <v>2</v>
+      </c>
+      <c r="D187" s="19">
+        <v>1</v>
+      </c>
+      <c r="E187" s="21">
+        <v>7</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G187" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A188" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B188" s="11">
+        <v>3</v>
+      </c>
+      <c r="C188" s="11">
+        <v>2</v>
+      </c>
+      <c r="D188" s="20">
+        <v>1</v>
+      </c>
+      <c r="E188" s="21">
+        <v>7</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G188" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A189" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B189" s="11">
+        <v>3</v>
+      </c>
+      <c r="C189" s="11">
+        <v>2</v>
+      </c>
+      <c r="D189" s="20">
+        <v>1</v>
+      </c>
+      <c r="E189" s="21">
+        <v>7</v>
+      </c>
+      <c r="F189" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G189" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A190" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B190" s="11">
+        <v>3</v>
+      </c>
+      <c r="C190" s="11">
+        <v>0</v>
+      </c>
+      <c r="D190" s="20">
+        <v>3</v>
+      </c>
+      <c r="E190" s="21">
+        <v>7</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G190" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A191" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B191" s="11">
+        <v>3</v>
+      </c>
+      <c r="C191" s="11">
+        <v>2</v>
+      </c>
+      <c r="D191" s="20">
+        <v>1</v>
+      </c>
+      <c r="E191" s="21">
+        <v>7</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G191" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A192" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B192" s="11">
+        <v>3</v>
+      </c>
+      <c r="C192" s="11">
+        <v>2</v>
+      </c>
+      <c r="D192" s="20">
+        <v>1</v>
+      </c>
+      <c r="E192" s="21">
+        <v>7</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G192" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A193" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B193" s="11">
+        <v>3</v>
+      </c>
+      <c r="C193" s="11">
+        <v>2</v>
+      </c>
+      <c r="D193" s="20">
+        <v>1</v>
+      </c>
+      <c r="E193" s="21">
+        <v>7</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G193" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A194" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B194" s="11">
+        <v>3</v>
+      </c>
+      <c r="C194" s="11">
+        <v>2</v>
+      </c>
+      <c r="D194" s="20">
+        <v>1</v>
+      </c>
+      <c r="E194" s="21">
+        <v>7</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G194" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A195" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B195" s="11">
+        <v>3</v>
+      </c>
+      <c r="C195" s="11">
+        <v>2</v>
+      </c>
+      <c r="D195" s="20">
+        <v>1</v>
+      </c>
+      <c r="E195" s="21">
+        <v>7</v>
+      </c>
+      <c r="F195" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G195" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A196" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B196" s="11">
+        <v>3</v>
+      </c>
+      <c r="C196" s="11">
+        <v>2</v>
+      </c>
+      <c r="D196" s="11">
+        <v>1</v>
+      </c>
+      <c r="E196" s="15">
+        <v>8</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G196" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A197" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B197" s="11">
+        <v>3</v>
+      </c>
+      <c r="C197" s="11">
+        <v>0</v>
+      </c>
+      <c r="D197" s="11">
+        <v>3</v>
+      </c>
+      <c r="E197" s="22">
+        <v>8</v>
+      </c>
+      <c r="F197" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G197" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A198" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B198" s="11">
+        <v>7</v>
+      </c>
+      <c r="C198" s="11">
+        <v>0</v>
+      </c>
+      <c r="D198" s="11">
+        <v>7</v>
+      </c>
+      <c r="E198" s="15">
+        <v>8</v>
+      </c>
+      <c r="F198" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G198" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A199" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B199" s="11">
+        <v>3</v>
+      </c>
+      <c r="C199" s="11">
+        <v>2</v>
+      </c>
+      <c r="D199" s="11">
+        <v>1</v>
+      </c>
+      <c r="E199" s="15">
+        <v>8</v>
+      </c>
+      <c r="F199" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G199" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A200" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B200" s="11">
+        <v>4</v>
+      </c>
+      <c r="C200" s="11">
+        <v>2</v>
+      </c>
+      <c r="D200" s="11">
+        <v>2</v>
+      </c>
+      <c r="E200" s="22">
+        <v>8</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G200" s="23" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>